<commit_message>
final clean-up for submission
</commit_message>
<xml_diff>
--- a/data/sample_list.xlsx
+++ b/data/sample_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18204"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="344">
   <si>
     <t>Sample</t>
   </si>
@@ -686,6 +686,9 @@
     <t>PA93a_11-46_5min_4a_20151113.raw</t>
   </si>
   <si>
+    <t>originally mis-labeled as 5min</t>
+  </si>
+  <si>
     <t>PA93b</t>
   </si>
   <si>
@@ -732,6 +735,9 @@
   </si>
   <si>
     <t>PA97a_11-46_1min_4a_20151113.raw</t>
+  </si>
+  <si>
+    <t>originally mis-labeled as 1min</t>
   </si>
   <si>
     <t>PA97b</t>
@@ -1133,20 +1139,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1555,8 +1561,8 @@
   <dimension ref="A1:L156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="D128" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="L157" sqref="L157"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="M107" sqref="M107"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -4623,7 +4629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>210</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>212</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>214</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>216</v>
       </c>
@@ -4733,7 +4739,7 @@
         <v>217</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>16</v>
@@ -4750,10 +4756,13 @@
       <c r="K100" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="101" spans="1:11">
+      <c r="L100" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B101" t="s">
         <v>13</v>
@@ -4765,13 +4774,13 @@
         <v>217</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>89</v>
@@ -4782,10 +4791,13 @@
       <c r="K101" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="102" spans="1:11">
+      <c r="L101" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B102" t="s">
         <v>13</v>
@@ -4803,7 +4815,7 @@
         <v>16</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>89</v>
@@ -4815,9 +4827,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B103" t="s">
         <v>13</v>
@@ -4835,7 +4847,7 @@
         <v>16</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>89</v>
@@ -4847,9 +4859,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B104" t="s">
         <v>13</v>
@@ -4867,7 +4879,7 @@
         <v>16</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>89</v>
@@ -4879,9 +4891,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B105" t="s">
         <v>13</v>
@@ -4899,7 +4911,7 @@
         <v>16</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>89</v>
@@ -4911,9 +4923,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B106" t="s">
         <v>13</v>
@@ -4931,7 +4943,7 @@
         <v>16</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>89</v>
@@ -4943,9 +4955,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B107" t="s">
         <v>13</v>
@@ -4963,7 +4975,7 @@
         <v>16</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>89</v>
@@ -4975,9 +4987,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B108" t="s">
         <v>13</v>
@@ -4989,13 +5001,13 @@
         <v>217</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>89</v>
@@ -5006,10 +5018,13 @@
       <c r="K108" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="109" spans="1:11">
+      <c r="L108" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B109" t="s">
         <v>13</v>
@@ -5021,13 +5036,13 @@
         <v>217</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>89</v>
@@ -5038,10 +5053,13 @@
       <c r="K109" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="110" spans="1:11">
+      <c r="L109" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B110" t="s">
         <v>13</v>
@@ -5059,7 +5077,7 @@
         <v>16</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>89</v>
@@ -5071,9 +5089,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B111" t="s">
         <v>13</v>
@@ -5091,7 +5109,7 @@
         <v>16</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>89</v>
@@ -5103,9 +5121,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B112" t="s">
         <v>13</v>
@@ -5123,7 +5141,7 @@
         <v>16</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>89</v>
@@ -5137,7 +5155,7 @@
     </row>
     <row r="113" spans="1:11">
       <c r="A113" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B113" t="s">
         <v>13</v>
@@ -5155,7 +5173,7 @@
         <v>16</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>89</v>
@@ -5169,7 +5187,7 @@
     </row>
     <row r="114" spans="1:11">
       <c r="A114" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B114" t="s">
         <v>13</v>
@@ -5187,7 +5205,7 @@
         <v>16</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>89</v>
@@ -5201,7 +5219,7 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B115" t="s">
         <v>13</v>
@@ -5219,7 +5237,7 @@
         <v>16</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>89</v>
@@ -5233,7 +5251,7 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B116" t="s">
         <v>13</v>
@@ -5251,7 +5269,7 @@
         <v>16</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>89</v>
@@ -5265,7 +5283,7 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B117" t="s">
         <v>13</v>
@@ -5283,7 +5301,7 @@
         <v>16</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>89</v>
@@ -5297,7 +5315,7 @@
     </row>
     <row r="118" spans="1:11">
       <c r="A118" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B118" t="s">
         <v>13</v>
@@ -5315,7 +5333,7 @@
         <v>16</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>89</v>
@@ -5326,7 +5344,7 @@
     </row>
     <row r="119" spans="1:11">
       <c r="A119" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B119" t="s">
         <v>13</v>
@@ -5344,7 +5362,7 @@
         <v>16</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>89</v>
@@ -5355,7 +5373,7 @@
     </row>
     <row r="120" spans="1:11">
       <c r="A120" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B120" t="s">
         <v>13</v>
@@ -5373,7 +5391,7 @@
         <v>16</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>89</v>
@@ -5384,7 +5402,7 @@
     </row>
     <row r="121" spans="1:11">
       <c r="A121" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B121" t="s">
         <v>13</v>
@@ -5402,7 +5420,7 @@
         <v>16</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>89</v>
@@ -5411,12 +5429,12 @@
         <v>42415</v>
       </c>
       <c r="K121" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="122" spans="1:11">
       <c r="A122" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B122" t="s">
         <v>13</v>
@@ -5434,7 +5452,7 @@
         <v>16</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>89</v>
@@ -5445,7 +5463,7 @@
     </row>
     <row r="123" spans="1:11">
       <c r="A123" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B123" t="s">
         <v>13</v>
@@ -5463,7 +5481,7 @@
         <v>16</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>89</v>
@@ -5474,7 +5492,7 @@
     </row>
     <row r="124" spans="1:11">
       <c r="A124" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B124" t="s">
         <v>13</v>
@@ -5492,7 +5510,7 @@
         <v>16</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>89</v>
@@ -5503,7 +5521,7 @@
     </row>
     <row r="125" spans="1:11">
       <c r="A125" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B125" t="s">
         <v>13</v>
@@ -5521,7 +5539,7 @@
         <v>16</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>89</v>
@@ -5532,7 +5550,7 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B126" t="s">
         <v>13</v>
@@ -5550,7 +5568,7 @@
         <v>16</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>89</v>
@@ -5561,7 +5579,7 @@
     </row>
     <row r="127" spans="1:11">
       <c r="A127" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B127" t="s">
         <v>13</v>
@@ -5579,7 +5597,7 @@
         <v>16</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>89</v>
@@ -5590,7 +5608,7 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B128" t="s">
         <v>13</v>
@@ -5608,7 +5626,7 @@
         <v>16</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>89</v>
@@ -5617,12 +5635,12 @@
         <v>42430</v>
       </c>
       <c r="K128" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:11">
       <c r="A129" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B129" t="s">
         <v>13</v>
@@ -5640,7 +5658,7 @@
         <v>16</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="H129" s="1" t="s">
         <v>89</v>
@@ -5651,7 +5669,7 @@
     </row>
     <row r="130" spans="1:11">
       <c r="A130" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B130" t="s">
         <v>13</v>
@@ -5669,7 +5687,7 @@
         <v>16</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>89</v>
@@ -5680,7 +5698,7 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B131" t="s">
         <v>13</v>
@@ -5698,7 +5716,7 @@
         <v>16</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>89</v>
@@ -5709,7 +5727,7 @@
     </row>
     <row r="132" spans="1:11">
       <c r="A132" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B132" t="s">
         <v>13</v>
@@ -5727,7 +5745,7 @@
         <v>16</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>89</v>
@@ -5738,7 +5756,7 @@
     </row>
     <row r="133" spans="1:11">
       <c r="A133" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B133" t="s">
         <v>13</v>
@@ -5756,7 +5774,7 @@
         <v>16</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>89</v>
@@ -5767,7 +5785,7 @@
     </row>
     <row r="134" spans="1:11">
       <c r="A134" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B134" t="s">
         <v>13</v>
@@ -5785,7 +5803,7 @@
         <v>16</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>89</v>
@@ -5796,7 +5814,7 @@
     </row>
     <row r="135" spans="1:11">
       <c r="A135" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B135" t="s">
         <v>13</v>
@@ -5814,7 +5832,7 @@
         <v>16</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>89</v>
@@ -5825,7 +5843,7 @@
     </row>
     <row r="136" spans="1:11">
       <c r="A136" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B136" t="s">
         <v>13</v>
@@ -5843,7 +5861,7 @@
         <v>16</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>89</v>
@@ -5854,7 +5872,7 @@
     </row>
     <row r="137" spans="1:11">
       <c r="A137" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B137" t="s">
         <v>13</v>
@@ -5872,7 +5890,7 @@
         <v>16</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>89</v>
@@ -5883,7 +5901,7 @@
     </row>
     <row r="138" spans="1:11">
       <c r="A138" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B138" t="s">
         <v>13</v>
@@ -5901,7 +5919,7 @@
         <v>16</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H138" s="1" t="s">
         <v>89</v>
@@ -5912,7 +5930,7 @@
     </row>
     <row r="139" spans="1:11">
       <c r="A139" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B139" t="s">
         <v>13</v>
@@ -5930,7 +5948,7 @@
         <v>16</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>89</v>
@@ -5941,7 +5959,7 @@
     </row>
     <row r="140" spans="1:11">
       <c r="A140" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B140" t="s">
         <v>13</v>
@@ -5959,7 +5977,7 @@
         <v>16</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>89</v>
@@ -5970,7 +5988,7 @@
     </row>
     <row r="141" spans="1:11">
       <c r="A141" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B141" t="s">
         <v>13</v>
@@ -5988,7 +6006,7 @@
         <v>16</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H141" s="1" t="s">
         <v>89</v>
@@ -5997,12 +6015,12 @@
         <v>42426</v>
       </c>
       <c r="K141" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="142" spans="1:11">
       <c r="A142" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B142" t="s">
         <v>13</v>
@@ -6020,7 +6038,7 @@
         <v>16</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>89</v>
@@ -6029,12 +6047,12 @@
         <v>42426</v>
       </c>
       <c r="K142" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="143" spans="1:11">
       <c r="A143" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B143" t="s">
         <v>13</v>
@@ -6052,7 +6070,7 @@
         <v>16</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>89</v>
@@ -6063,7 +6081,7 @@
     </row>
     <row r="144" spans="1:11">
       <c r="A144" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B144" t="s">
         <v>13</v>
@@ -6081,7 +6099,7 @@
         <v>16</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>89</v>
@@ -6092,7 +6110,7 @@
     </row>
     <row r="145" spans="1:12">
       <c r="A145" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B145" t="s">
         <v>13</v>
@@ -6110,7 +6128,7 @@
         <v>16</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>89</v>
@@ -6121,7 +6139,7 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B146" t="s">
         <v>13</v>
@@ -6139,7 +6157,7 @@
         <v>16</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>89</v>
@@ -6148,12 +6166,12 @@
         <v>42425</v>
       </c>
       <c r="K146" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B147" t="s">
         <v>13</v>
@@ -6171,7 +6189,7 @@
         <v>16</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>89</v>
@@ -6180,12 +6198,12 @@
         <v>42425</v>
       </c>
       <c r="K147" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B148" t="s">
         <v>13</v>
@@ -6203,7 +6221,7 @@
         <v>16</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>89</v>
@@ -6214,7 +6232,7 @@
     </row>
     <row r="149" spans="1:12">
       <c r="A149" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B149" t="s">
         <v>13</v>
@@ -6232,7 +6250,7 @@
         <v>16</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>89</v>
@@ -6243,7 +6261,7 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B150" t="s">
         <v>13</v>
@@ -6261,7 +6279,7 @@
         <v>16</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>89</v>
@@ -6272,7 +6290,7 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B151" t="s">
         <v>13</v>
@@ -6290,7 +6308,7 @@
         <v>16</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>89</v>
@@ -6299,12 +6317,12 @@
         <v>42431</v>
       </c>
       <c r="K151" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B152" t="s">
         <v>13</v>
@@ -6322,7 +6340,7 @@
         <v>16</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>89</v>
@@ -6331,12 +6349,12 @@
         <v>42431</v>
       </c>
       <c r="K152" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="153" spans="1:12">
       <c r="A153" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B153" t="s">
         <v>13</v>
@@ -6348,21 +6366,21 @@
         <v>16</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="K153" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L153" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B154" t="s">
         <v>13</v>
@@ -6374,21 +6392,21 @@
         <v>16</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="K154" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="L154" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B155" t="s">
         <v>13</v>
@@ -6397,21 +6415,21 @@
         <v>16</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="K155" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L155" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B156" t="s">
         <v>13</v>
@@ -6420,16 +6438,16 @@
         <v>16</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="K156" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="L156" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>